<commit_message>
first git commit for my selenium code
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdata/selenium.xlsx
+++ b/src/main/resources/Testdata/selenium.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7830" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7830" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
     <sheet name="Productdetails" sheetId="2" r:id="rId2"/>
+    <sheet name="NewRegistration" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t xml:space="preserve">username </t>
   </si>
@@ -63,17 +64,84 @@
   </si>
   <si>
     <t>White</t>
+  </si>
+  <si>
+    <t>NewMailid</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Pincode</t>
+  </si>
+  <si>
+    <t>MobileNum</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>venkatmuppidi10@gmail.com</t>
+  </si>
+  <si>
+    <t>Mr.</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Password@2020</t>
+  </si>
+  <si>
+    <t>Main road</t>
+  </si>
+  <si>
+    <t>hyd</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>32003</t>
+  </si>
+  <si>
+    <t>9876543210</t>
+  </si>
+  <si>
+    <t>23/12/1993</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -92,9 +160,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -102,28 +184,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -161,15 +221,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -177,21 +247,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -205,24 +260,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -237,19 +305,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -261,163 +473,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -428,21 +496,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -496,9 +549,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -520,165 +590,167 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1019,10 +1091,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1041,7 +1113,7 @@
   <sheetPr/>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -1106,4 +1178,104 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="30.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="10.8571428571429" customWidth="1"/>
+    <col min="4" max="4" width="12.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="16.5714285714286" customWidth="1"/>
+    <col min="6" max="6" width="10.4285714285714" customWidth="1"/>
+    <col min="10" max="10" width="12.4285714285714" customWidth="1"/>
+    <col min="11" max="11" width="11.1428571428571"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="Password@2020"/>
+    <hyperlink ref="A2" r:id="rId2" display="venkatmuppidi10@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modification done on script
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdata/selenium.xlsx
+++ b/src/main/resources/Testdata/selenium.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7830" activeTab="2"/>
+    <workbookView windowWidth="20490" windowHeight="7830" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t xml:space="preserve">username </t>
   </si>
@@ -51,12 +51,15 @@
     <t>M</t>
   </si>
   <si>
-    <t>Yellow</t>
+    <t>Orange</t>
   </si>
   <si>
     <t>Product successfully added to your shopping cart</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>Blouse</t>
   </si>
   <si>
@@ -64,6 +67,9 @@
   </si>
   <si>
     <t>White</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
   <si>
     <t>NewMailid</t>
@@ -168,22 +174,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -197,11 +195,41 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -213,9 +241,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -229,17 +271,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -259,42 +301,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -305,73 +311,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -384,108 +492,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,15 +529,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -549,11 +546,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -569,6 +564,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -591,15 +597,15 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -617,138 +623,137 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1"/>
   </cellXfs>
@@ -1091,10 +1096,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1113,8 +1118,8 @@
   <sheetPr/>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="4"/>
@@ -1153,25 +1158,25 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="E2">
-        <v>1</v>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="E3">
-        <v>2</v>
+      <c r="E3" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1185,7 +1190,7 @@
   <sheetPr/>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -1202,72 +1207,72 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="I2" s="3" t="s">
         <v>37</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated code with new Assessment
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdata/selenium.xlsx
+++ b/src/main/resources/Testdata/selenium.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7830" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7830" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t xml:space="preserve">username </t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>DOB</t>
-  </si>
-  <si>
-    <t>venkatmuppidi10@gmail.com</t>
   </si>
   <si>
     <t>Mr.</t>
@@ -143,11 +140,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -167,21 +164,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -195,39 +200,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -241,6 +232,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -248,47 +277,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -301,6 +291,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -311,12 +308,108 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -329,13 +422,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -347,49 +464,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -407,85 +482,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -505,17 +502,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -544,11 +537,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -570,26 +584,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -605,15 +602,15 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -623,139 +620,139 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1078,7 +1075,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1118,7 +1115,7 @@
   <sheetPr/>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1190,8 +1187,8 @@
   <sheetPr/>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1242,43 +1239,43 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>29</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>31</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" t="s">
         <v>33</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>34</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>35</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="Password@2020"/>
-    <hyperlink ref="A2" r:id="rId2" display="venkatmuppidi10@gmail.com"/>
+    <hyperlink ref="A2" r:id="rId2" display="venkatklu1993@gmail.com" tooltip="mailto:venkatklu1993@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>